<commit_message>
Create classes to manage load and storage the data
</commit_message>
<xml_diff>
--- a/data/Bancomer.xlsx
+++ b/data/Bancomer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerashdo/programming/python/payments-project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4EE418-F469-9845-BCF9-F9C039D98DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDC6CB9-BFAC-9744-873C-D45F83124364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{5FC76A27-4442-714B-8100-E28315A3B639}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{5FC76A27-4442-714B-8100-E28315A3B639}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>